<commit_message>
Cambio toneladas por día India
</commit_message>
<xml_diff>
--- a/data/india/total_bmw_waste.xlsx
+++ b/data/india/total_bmw_waste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\plastics-COVID_project\data\india\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B96D7D1-514B-4B36-9400-2D3CB0258C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8190C0A6-4333-433C-A0E9-02EBAD257AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B4E174C-A9DA-4493-A8B8-40B33161D33A}"/>
   </bookViews>
@@ -34,43 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>ENERO</t>
-  </si>
-  <si>
-    <t>FEBRERO</t>
-  </si>
-  <si>
-    <t>MARZO</t>
-  </si>
-  <si>
-    <t>ABRIL</t>
-  </si>
-  <si>
-    <t>MAYO</t>
-  </si>
-  <si>
-    <t>JUNIO</t>
-  </si>
-  <si>
-    <t>JULIO</t>
-  </si>
-  <si>
-    <t>AGOSTO</t>
-  </si>
-  <si>
-    <t>SEPTIEMBRE</t>
-  </si>
-  <si>
-    <t>OCTUBRE</t>
-  </si>
-  <si>
-    <t>NOVIEMBRE</t>
-  </si>
-  <si>
-    <t>DICIEMBRE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>3025.41</t>
   </si>
@@ -85,6 +49,12 @@
   </si>
   <si>
     <t>4527.55</t>
+  </si>
+  <si>
+    <t>FECHA</t>
+  </si>
+  <si>
+    <t>TPD</t>
   </si>
 </sst>
 </file>
@@ -130,11 +100,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,108 +420,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8731E02A-8168-428A-86F5-993FFAEA4B63}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1">
-        <v>2020</v>
-      </c>
-      <c r="C1">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B5">
+        <v>5490</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>44105</v>
+      </c>
+      <c r="B6">
+        <v>5597</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>44136</v>
+      </c>
+      <c r="B7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>44166</v>
+      </c>
+      <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B9">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>44228</v>
+      </c>
+      <c r="B10">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>44256</v>
+      </c>
+      <c r="B11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>44287</v>
+      </c>
+      <c r="B12">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>44317</v>
+      </c>
+      <c r="B13">
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>44348</v>
+      </c>
+      <c r="B14">
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>5490</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>5597</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Modificación toneladas por día a toneladas totales
</commit_message>
<xml_diff>
--- a/data/india/total_bmw_waste.xlsx
+++ b/data/india/total_bmw_waste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\plastics-COVID_project\data\india\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8190C0A6-4333-433C-A0E9-02EBAD257AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651DC2DA-DF46-41F9-9E1C-EF32DBC45A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B4E174C-A9DA-4493-A8B8-40B33161D33A}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +497,8 @@
         <v>44197</v>
       </c>
       <c r="B9">
-        <v>74</v>
+        <f>74*31</f>
+        <v>2294</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -505,7 +506,8 @@
         <v>44228</v>
       </c>
       <c r="B10">
-        <v>53</v>
+        <f>53*28</f>
+        <v>1484</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -513,7 +515,8 @@
         <v>44256</v>
       </c>
       <c r="B11">
-        <v>75</v>
+        <f>75*31</f>
+        <v>2325</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -521,7 +524,8 @@
         <v>44287</v>
       </c>
       <c r="B12">
-        <v>139</v>
+        <f>139*30</f>
+        <v>4170</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -529,7 +533,8 @@
         <v>44317</v>
       </c>
       <c r="B13">
-        <v>203</v>
+        <f>203*31</f>
+        <v>6293</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -537,7 +542,8 @@
         <v>44348</v>
       </c>
       <c r="B14">
-        <v>164</v>
+        <f>164*30</f>
+        <v>4920</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se añadió total BMW por estado
</commit_message>
<xml_diff>
--- a/data/india/total_bmw_waste.xlsx
+++ b/data/india/total_bmw_waste.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\plastics-COVID_project\data\india\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DescargasChrome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651DC2DA-DF46-41F9-9E1C-EF32DBC45A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CB0AF4-A444-46EF-B48A-8E2BA079690B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B4E174C-A9DA-4493-A8B8-40B33161D33A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4B4E174C-A9DA-4493-A8B8-40B33161D33A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>3025.41</t>
   </si>
@@ -55,6 +56,114 @@
   </si>
   <si>
     <t>TPD</t>
+  </si>
+  <si>
+    <t>Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>Assam</t>
+  </si>
+  <si>
+    <t>Bihar</t>
+  </si>
+  <si>
+    <t>Chandigarh</t>
+  </si>
+  <si>
+    <t>Chhattisgarh</t>
+  </si>
+  <si>
+    <t>DD &amp; DNH</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Gujarat</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>Himachal Pradesh</t>
+  </si>
+  <si>
+    <t>Jammu and Kashmir</t>
+  </si>
+  <si>
+    <t>Jharkhand</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>Lakshadweep</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Madhya Pradesh</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>Manipur</t>
+  </si>
+  <si>
+    <t>Meghalaya</t>
+  </si>
+  <si>
+    <t>Odisha</t>
+  </si>
+  <si>
+    <t>Puducherry</t>
+  </si>
+  <si>
+    <t>Punjab</t>
+  </si>
+  <si>
+    <t>Rajasthan</t>
+  </si>
+  <si>
+    <t>Sikkim</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>Telangana</t>
+  </si>
+  <si>
+    <t>Tripura</t>
+  </si>
+  <si>
+    <t>Uttarakhand</t>
+  </si>
+  <si>
+    <t>Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>West Bengal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andaman &amp; Nicobar </t>
+  </si>
+  <si>
+    <t>Arunachal Pradesh</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>Mizoram</t>
+  </si>
+  <si>
+    <t>Nagaland</t>
   </si>
 </sst>
 </file>
@@ -422,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8731E02A-8168-428A-86F5-993FFAEA4B63}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,4 +674,1100 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15A2A4F-ADDD-4801-931F-B7955909B94A}">
+  <dimension ref="A1:AJ14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B2">
+        <v>0.42</v>
+      </c>
+      <c r="C2">
+        <v>165.48</v>
+      </c>
+      <c r="D2">
+        <v>3.36</v>
+      </c>
+      <c r="E2">
+        <v>28.38</v>
+      </c>
+      <c r="F2">
+        <v>6.84</v>
+      </c>
+      <c r="G2">
+        <v>29.85</v>
+      </c>
+      <c r="H2">
+        <v>11.19</v>
+      </c>
+      <c r="J2">
+        <v>333.42</v>
+      </c>
+      <c r="K2">
+        <v>0.81</v>
+      </c>
+      <c r="L2">
+        <v>350.79</v>
+      </c>
+      <c r="M2">
+        <v>75.33</v>
+      </c>
+      <c r="N2">
+        <v>3.81</v>
+      </c>
+      <c r="O2">
+        <v>10.71</v>
+      </c>
+      <c r="Q2">
+        <v>84</v>
+      </c>
+      <c r="R2">
+        <v>141.30000000000001</v>
+      </c>
+      <c r="S2">
+        <v>0.3</v>
+      </c>
+      <c r="T2">
+        <v>224.58</v>
+      </c>
+      <c r="U2">
+        <v>524.82000000000005</v>
+      </c>
+      <c r="V2">
+        <v>5.13</v>
+      </c>
+      <c r="W2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="X2">
+        <v>4.2</v>
+      </c>
+      <c r="Y2">
+        <v>3.6</v>
+      </c>
+      <c r="Z2">
+        <v>31.86</v>
+      </c>
+      <c r="AA2">
+        <v>18.63</v>
+      </c>
+      <c r="AB2">
+        <v>48</v>
+      </c>
+      <c r="AC2">
+        <v>177</v>
+      </c>
+      <c r="AD2">
+        <v>6</v>
+      </c>
+      <c r="AE2">
+        <v>312.3</v>
+      </c>
+      <c r="AF2">
+        <v>12.3</v>
+      </c>
+      <c r="AG2">
+        <v>0.45</v>
+      </c>
+      <c r="AH2">
+        <v>0.45</v>
+      </c>
+      <c r="AI2">
+        <v>210</v>
+      </c>
+      <c r="AJ2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44013</v>
+      </c>
+      <c r="C3">
+        <v>182.81</v>
+      </c>
+      <c r="D3">
+        <v>3.36</v>
+      </c>
+      <c r="E3">
+        <v>20.68</v>
+      </c>
+      <c r="F3">
+        <v>20.76</v>
+      </c>
+      <c r="G3">
+        <v>5.65</v>
+      </c>
+      <c r="J3">
+        <v>389.58</v>
+      </c>
+      <c r="K3">
+        <v>0.81</v>
+      </c>
+      <c r="L3">
+        <v>306.14</v>
+      </c>
+      <c r="M3">
+        <v>184.18</v>
+      </c>
+      <c r="N3">
+        <v>12.5</v>
+      </c>
+      <c r="O3">
+        <v>9.77</v>
+      </c>
+      <c r="Q3">
+        <v>540.28</v>
+      </c>
+      <c r="R3">
+        <v>293.32</v>
+      </c>
+      <c r="T3">
+        <v>56.4</v>
+      </c>
+      <c r="U3">
+        <v>1180</v>
+      </c>
+      <c r="V3">
+        <v>0.2</v>
+      </c>
+      <c r="W3">
+        <v>1.74</v>
+      </c>
+      <c r="Y3">
+        <v>3.4</v>
+      </c>
+      <c r="Z3">
+        <v>106.63</v>
+      </c>
+      <c r="AA3">
+        <v>35.82</v>
+      </c>
+      <c r="AB3">
+        <v>35.590000000000003</v>
+      </c>
+      <c r="AC3">
+        <v>7.15</v>
+      </c>
+      <c r="AD3">
+        <v>0.2</v>
+      </c>
+      <c r="AE3">
+        <v>401.29</v>
+      </c>
+      <c r="AF3">
+        <v>10.5</v>
+      </c>
+      <c r="AH3">
+        <v>0.82</v>
+      </c>
+      <c r="AI3">
+        <v>307.54000000000002</v>
+      </c>
+      <c r="AJ3">
+        <v>136.37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>44044</v>
+      </c>
+      <c r="C4">
+        <v>118.82</v>
+      </c>
+      <c r="D4">
+        <v>3.8</v>
+      </c>
+      <c r="E4">
+        <v>12.57</v>
+      </c>
+      <c r="F4">
+        <v>41.54</v>
+      </c>
+      <c r="G4">
+        <v>55.34</v>
+      </c>
+      <c r="H4">
+        <v>13.39</v>
+      </c>
+      <c r="J4">
+        <v>296.14</v>
+      </c>
+      <c r="L4">
+        <v>360.04</v>
+      </c>
+      <c r="M4">
+        <v>210.69</v>
+      </c>
+      <c r="N4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="O4">
+        <v>51.77</v>
+      </c>
+      <c r="P4">
+        <v>2.59</v>
+      </c>
+      <c r="Q4">
+        <v>588.03</v>
+      </c>
+      <c r="R4">
+        <v>588.04999999999995</v>
+      </c>
+      <c r="S4" t="s">
+        <v>22</v>
+      </c>
+      <c r="T4">
+        <v>106.59</v>
+      </c>
+      <c r="U4">
+        <v>1359</v>
+      </c>
+      <c r="V4">
+        <v>2.09</v>
+      </c>
+      <c r="W4">
+        <v>6.34</v>
+      </c>
+      <c r="Y4">
+        <v>3.1</v>
+      </c>
+      <c r="Z4">
+        <v>109.19</v>
+      </c>
+      <c r="AA4">
+        <v>41.54</v>
+      </c>
+      <c r="AB4">
+        <v>21.19</v>
+      </c>
+      <c r="AC4">
+        <v>50.43</v>
+      </c>
+      <c r="AD4">
+        <v>0.3</v>
+      </c>
+      <c r="AE4">
+        <v>481.1</v>
+      </c>
+      <c r="AF4">
+        <v>24.04</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>41.85</v>
+      </c>
+      <c r="AI4">
+        <v>408.86</v>
+      </c>
+      <c r="AJ4">
+        <v>235.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B5">
+        <v>0.42</v>
+      </c>
+      <c r="C5">
+        <v>112.35</v>
+      </c>
+      <c r="D5">
+        <v>3.36</v>
+      </c>
+      <c r="E5">
+        <v>62.61</v>
+      </c>
+      <c r="F5">
+        <v>45.36</v>
+      </c>
+      <c r="G5">
+        <v>43.02</v>
+      </c>
+      <c r="H5">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I5">
+        <v>0.48</v>
+      </c>
+      <c r="J5">
+        <v>382.5</v>
+      </c>
+      <c r="K5">
+        <v>15</v>
+      </c>
+      <c r="L5">
+        <v>622.89</v>
+      </c>
+      <c r="M5">
+        <v>278.31</v>
+      </c>
+      <c r="N5">
+        <v>25.2</v>
+      </c>
+      <c r="O5">
+        <v>57.39</v>
+      </c>
+      <c r="P5">
+        <v>4.8</v>
+      </c>
+      <c r="Q5">
+        <v>168</v>
+      </c>
+      <c r="R5">
+        <v>494.1</v>
+      </c>
+      <c r="S5">
+        <v>0.3</v>
+      </c>
+      <c r="T5">
+        <v>339</v>
+      </c>
+      <c r="U5">
+        <v>524.82000000000005</v>
+      </c>
+      <c r="V5">
+        <v>5.13</v>
+      </c>
+      <c r="W5">
+        <v>9.9</v>
+      </c>
+      <c r="X5">
+        <v>4.2</v>
+      </c>
+      <c r="Y5">
+        <v>2.85</v>
+      </c>
+      <c r="Z5">
+        <v>134.01</v>
+      </c>
+      <c r="AA5">
+        <v>63</v>
+      </c>
+      <c r="AB5">
+        <v>234.42</v>
+      </c>
+      <c r="AC5">
+        <v>145.08000000000001</v>
+      </c>
+      <c r="AD5">
+        <v>6</v>
+      </c>
+      <c r="AE5">
+        <v>543.78</v>
+      </c>
+      <c r="AF5">
+        <v>188.82</v>
+      </c>
+      <c r="AG5">
+        <v>0.45</v>
+      </c>
+      <c r="AH5">
+        <v>21.72</v>
+      </c>
+      <c r="AI5">
+        <v>507.15</v>
+      </c>
+      <c r="AJ5">
+        <v>434.76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>44105</v>
+      </c>
+      <c r="B6">
+        <v>0.434</v>
+      </c>
+      <c r="C6">
+        <v>116.095</v>
+      </c>
+      <c r="D6">
+        <v>3.472</v>
+      </c>
+      <c r="E6">
+        <v>51.738999999999997</v>
+      </c>
+      <c r="F6">
+        <v>44.64</v>
+      </c>
+      <c r="G6">
+        <v>73.191000000000003</v>
+      </c>
+      <c r="H6">
+        <v>9.61</v>
+      </c>
+      <c r="I6">
+        <v>2.387</v>
+      </c>
+      <c r="J6">
+        <v>365.89299999999997</v>
+      </c>
+      <c r="K6">
+        <v>7.75</v>
+      </c>
+      <c r="L6">
+        <v>545.87900000000002</v>
+      </c>
+      <c r="M6">
+        <v>238.452</v>
+      </c>
+      <c r="N6">
+        <v>28.117000000000001</v>
+      </c>
+      <c r="O6">
+        <v>59.302999999999997</v>
+      </c>
+      <c r="P6">
+        <v>4.96</v>
+      </c>
+      <c r="Q6">
+        <v>218.023</v>
+      </c>
+      <c r="R6">
+        <v>641.97900000000004</v>
+      </c>
+      <c r="S6">
+        <v>0.31</v>
+      </c>
+      <c r="T6">
+        <v>308.41899999999998</v>
+      </c>
+      <c r="U6">
+        <v>542.31399999999996</v>
+      </c>
+      <c r="V6">
+        <v>5.3010000000000002</v>
+      </c>
+      <c r="W6">
+        <v>12.028</v>
+      </c>
+      <c r="X6">
+        <v>3.2240000000000002</v>
+      </c>
+      <c r="Y6">
+        <v>3.3170000000000002</v>
+      </c>
+      <c r="Z6">
+        <v>183.458</v>
+      </c>
+      <c r="AA6">
+        <v>58.652000000000001</v>
+      </c>
+      <c r="AB6">
+        <v>149.60599999999999</v>
+      </c>
+      <c r="AC6">
+        <v>171.554</v>
+      </c>
+      <c r="AD6">
+        <v>4.2160000000000002</v>
+      </c>
+      <c r="AE6">
+        <v>524.17899999999997</v>
+      </c>
+      <c r="AF6">
+        <v>144.80099999999999</v>
+      </c>
+      <c r="AG6">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="AH6">
+        <v>108.996</v>
+      </c>
+      <c r="AI6">
+        <v>478.08199999999999</v>
+      </c>
+      <c r="AJ6">
+        <v>486.79300000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>44136</v>
+      </c>
+      <c r="B7">
+        <v>0.42</v>
+      </c>
+      <c r="C7">
+        <v>317.91000000000003</v>
+      </c>
+      <c r="D7">
+        <v>3.36</v>
+      </c>
+      <c r="E7">
+        <v>50.07</v>
+      </c>
+      <c r="F7">
+        <v>28.08</v>
+      </c>
+      <c r="G7">
+        <v>70.83</v>
+      </c>
+      <c r="H7">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I7">
+        <v>1.08</v>
+      </c>
+      <c r="J7">
+        <v>385.47</v>
+      </c>
+      <c r="K7">
+        <v>5.43</v>
+      </c>
+      <c r="L7">
+        <v>423.51</v>
+      </c>
+      <c r="M7">
+        <v>239.4</v>
+      </c>
+      <c r="N7">
+        <v>30.03</v>
+      </c>
+      <c r="O7">
+        <v>44.82</v>
+      </c>
+      <c r="P7">
+        <v>4.8</v>
+      </c>
+      <c r="Q7">
+        <v>210.99</v>
+      </c>
+      <c r="R7">
+        <v>600.39</v>
+      </c>
+      <c r="S7">
+        <v>0.3</v>
+      </c>
+      <c r="T7">
+        <v>208.65</v>
+      </c>
+      <c r="U7">
+        <v>609</v>
+      </c>
+      <c r="V7">
+        <v>5.13</v>
+      </c>
+      <c r="W7">
+        <v>7.65</v>
+      </c>
+      <c r="X7">
+        <v>3.12</v>
+      </c>
+      <c r="Y7">
+        <v>1.86</v>
+      </c>
+      <c r="Z7">
+        <v>222.66</v>
+      </c>
+      <c r="AA7">
+        <v>28.74</v>
+      </c>
+      <c r="AB7">
+        <v>96.51</v>
+      </c>
+      <c r="AC7">
+        <v>141.93</v>
+      </c>
+      <c r="AD7">
+        <v>3.69</v>
+      </c>
+      <c r="AE7">
+        <v>300.75</v>
+      </c>
+      <c r="AF7">
+        <v>103.89</v>
+      </c>
+      <c r="AG7">
+        <v>0.45</v>
+      </c>
+      <c r="AH7">
+        <v>56.76</v>
+      </c>
+      <c r="AI7">
+        <v>316.70999999999998</v>
+      </c>
+      <c r="AJ7">
+        <v>330.84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>44166</v>
+      </c>
+      <c r="B8">
+        <v>0.43</v>
+      </c>
+      <c r="C8">
+        <v>328.51</v>
+      </c>
+      <c r="D8">
+        <v>3.47</v>
+      </c>
+      <c r="E8">
+        <v>23.41</v>
+      </c>
+      <c r="F8">
+        <v>23.31</v>
+      </c>
+      <c r="G8">
+        <v>73.19</v>
+      </c>
+      <c r="H8">
+        <v>9.61</v>
+      </c>
+      <c r="I8">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="J8">
+        <v>321.32</v>
+      </c>
+      <c r="K8">
+        <v>5.39</v>
+      </c>
+      <c r="L8">
+        <v>479.57</v>
+      </c>
+      <c r="M8">
+        <v>209.93</v>
+      </c>
+      <c r="N8">
+        <v>48.24</v>
+      </c>
+      <c r="O8">
+        <v>35.119999999999997</v>
+      </c>
+      <c r="P8">
+        <v>11.63</v>
+      </c>
+      <c r="Q8">
+        <v>218.02</v>
+      </c>
+      <c r="R8">
+        <v>542.47</v>
+      </c>
+      <c r="S8">
+        <v>0.31</v>
+      </c>
+      <c r="T8">
+        <v>249.49</v>
+      </c>
+      <c r="U8">
+        <v>629.29999999999995</v>
+      </c>
+      <c r="V8">
+        <v>9.27</v>
+      </c>
+      <c r="W8">
+        <v>8.56</v>
+      </c>
+      <c r="X8">
+        <v>3.22</v>
+      </c>
+      <c r="Y8">
+        <v>2.29</v>
+      </c>
+      <c r="Z8">
+        <v>125.58</v>
+      </c>
+      <c r="AA8">
+        <v>17.11</v>
+      </c>
+      <c r="AB8">
+        <v>86.99</v>
+      </c>
+      <c r="AC8">
+        <v>105.93</v>
+      </c>
+      <c r="AD8">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AE8">
+        <v>251.22</v>
+      </c>
+      <c r="AF8">
+        <v>68.819999999999993</v>
+      </c>
+      <c r="AG8">
+        <v>0.47</v>
+      </c>
+      <c r="AH8">
+        <v>76.260000000000005</v>
+      </c>
+      <c r="AI8">
+        <v>276.45999999999998</v>
+      </c>
+      <c r="AJ8">
+        <v>279.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>44228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>44287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>44317</v>
+      </c>
+      <c r="B13">
+        <v>0.434</v>
+      </c>
+      <c r="C13">
+        <v>309.69</v>
+      </c>
+      <c r="D13">
+        <v>3.472</v>
+      </c>
+      <c r="E13">
+        <v>16.12</v>
+      </c>
+      <c r="F13">
+        <v>32.86</v>
+      </c>
+      <c r="G13">
+        <v>59.21</v>
+      </c>
+      <c r="H13">
+        <v>85.559999999999988</v>
+      </c>
+      <c r="I13">
+        <v>2.0150000000000001</v>
+      </c>
+      <c r="J13">
+        <v>582.49</v>
+      </c>
+      <c r="K13">
+        <v>13.950000000000001</v>
+      </c>
+      <c r="L13">
+        <v>681.38</v>
+      </c>
+      <c r="M13">
+        <v>406.40999999999997</v>
+      </c>
+      <c r="N13">
+        <v>70.37</v>
+      </c>
+      <c r="O13">
+        <v>77.190000000000012</v>
+      </c>
+      <c r="P13">
+        <v>17.360000000000003</v>
+      </c>
+      <c r="Q13">
+        <v>524.21</v>
+      </c>
+      <c r="R13">
+        <v>735.01</v>
+      </c>
+      <c r="S13">
+        <v>0.31</v>
+      </c>
+      <c r="T13">
+        <v>226.92000000000002</v>
+      </c>
+      <c r="U13">
+        <v>589.62</v>
+      </c>
+      <c r="V13">
+        <v>4.03</v>
+      </c>
+      <c r="W13">
+        <v>7.75</v>
+      </c>
+      <c r="X13">
+        <v>1.0230000000000001</v>
+      </c>
+      <c r="Y13">
+        <v>2.294</v>
+      </c>
+      <c r="Z13">
+        <v>206.15</v>
+      </c>
+      <c r="AA13">
+        <v>56.11</v>
+      </c>
+      <c r="AB13">
+        <v>124</v>
+      </c>
+      <c r="AC13">
+        <v>154.38000000000002</v>
+      </c>
+      <c r="AD13">
+        <v>0.46499999999999997</v>
+      </c>
+      <c r="AE13">
+        <v>420.67</v>
+      </c>
+      <c r="AF13">
+        <v>153.76</v>
+      </c>
+      <c r="AG13">
+        <v>0.62</v>
+      </c>
+      <c r="AH13">
+        <v>61.38</v>
+      </c>
+      <c r="AI13">
+        <v>493.21</v>
+      </c>
+      <c r="AJ13">
+        <v>177.32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>44348</v>
+      </c>
+      <c r="B14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C14">
+        <v>11.96</v>
+      </c>
+      <c r="D14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E14">
+        <v>0.81</v>
+      </c>
+      <c r="F14">
+        <v>1.19</v>
+      </c>
+      <c r="G14">
+        <v>1.78</v>
+      </c>
+      <c r="H14">
+        <v>1.02</v>
+      </c>
+      <c r="I14">
+        <v>3.9E-2</v>
+      </c>
+      <c r="J14">
+        <v>7.68</v>
+      </c>
+      <c r="K14">
+        <v>0.88</v>
+      </c>
+      <c r="L14">
+        <v>5.48</v>
+      </c>
+      <c r="M14">
+        <v>5.04</v>
+      </c>
+      <c r="N14">
+        <v>2.14</v>
+      </c>
+      <c r="O14">
+        <v>1.82</v>
+      </c>
+      <c r="P14">
+        <v>0.83</v>
+      </c>
+      <c r="Q14">
+        <v>14.5</v>
+      </c>
+      <c r="R14">
+        <v>26.95</v>
+      </c>
+      <c r="S14">
+        <v>0.01</v>
+      </c>
+      <c r="T14">
+        <v>4.18</v>
+      </c>
+      <c r="U14">
+        <v>14.25</v>
+      </c>
+      <c r="V14">
+        <v>0.31</v>
+      </c>
+      <c r="W14">
+        <v>0.6</v>
+      </c>
+      <c r="X14">
+        <v>0.12</v>
+      </c>
+      <c r="Y14">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="Z14">
+        <v>9.14</v>
+      </c>
+      <c r="AA14">
+        <v>1.67</v>
+      </c>
+      <c r="AB14">
+        <v>3.87</v>
+      </c>
+      <c r="AC14">
+        <v>3.61</v>
+      </c>
+      <c r="AD14">
+        <v>0.21</v>
+      </c>
+      <c r="AE14">
+        <v>26.04</v>
+      </c>
+      <c r="AF14">
+        <v>5.24</v>
+      </c>
+      <c r="AG14">
+        <v>6.2E-2</v>
+      </c>
+      <c r="AH14">
+        <v>1.2</v>
+      </c>
+      <c r="AI14">
+        <v>4.38</v>
+      </c>
+      <c r="AJ14">
+        <v>7.06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cambiar formato de las fechas
</commit_message>
<xml_diff>
--- a/data/india/total_bmw_waste.xlsx
+++ b/data/india/total_bmw_waste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DescargasChrome\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A68C224-EBB2-4BC6-9DC0-D21A9F38ACC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{451844AA-71C2-4CFF-AE47-3B701E0EFD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4B4E174C-A9DA-4493-A8B8-40B33161D33A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>3025.41</t>
   </si>
@@ -161,6 +161,45 @@
   </si>
   <si>
     <t>Nagaland</t>
+  </si>
+  <si>
+    <t>2020-06</t>
+  </si>
+  <si>
+    <t>2020-07</t>
+  </si>
+  <si>
+    <t>2020-08</t>
+  </si>
+  <si>
+    <t>2020-09</t>
+  </si>
+  <si>
+    <t>2020-10</t>
+  </si>
+  <si>
+    <t>2020-11</t>
+  </si>
+  <si>
+    <t>2020-12</t>
+  </si>
+  <si>
+    <t>2021-01</t>
+  </si>
+  <si>
+    <t>2021-02</t>
+  </si>
+  <si>
+    <t>2021-03</t>
+  </si>
+  <si>
+    <t>2021-04</t>
+  </si>
+  <si>
+    <t>2021-05</t>
+  </si>
+  <si>
+    <t>2021-06</t>
   </si>
 </sst>
 </file>
@@ -678,7 +717,7 @@
   <dimension ref="A1:AJ14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,8 +836,8 @@
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>43983</v>
+      <c r="A2" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B2">
         <v>0.42</v>
@@ -901,8 +940,8 @@
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>44013</v>
+      <c r="A3" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C3">
         <v>182.81</v>
@@ -990,8 +1029,8 @@
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>44044</v>
+      <c r="A4" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C4">
         <v>118.82</v>
@@ -1082,8 +1121,8 @@
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>44075</v>
+      <c r="A5" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B5">
         <v>0.42</v>
@@ -1192,8 +1231,8 @@
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>44105</v>
+      <c r="A6" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B6">
         <v>0.434</v>
@@ -1302,8 +1341,8 @@
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>44136</v>
+      <c r="A7" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B7">
         <v>0.42</v>
@@ -1412,8 +1451,8 @@
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>44166</v>
+      <c r="A8" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="B8">
         <v>0.43</v>
@@ -1522,28 +1561,28 @@
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>44197</v>
+      <c r="A9" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>44228</v>
+      <c r="A10" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>44256</v>
+      <c r="A11" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>44287</v>
+      <c r="A12" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>44317</v>
+      <c r="A13" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="B13">
         <v>0.434</v>
@@ -1652,8 +1691,8 @@
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>44348</v>
+      <c r="A14" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="B14">
         <v>3.0000000000000001E-3</v>
@@ -1762,6 +1801,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregar toneladas por día a Puducherry
</commit_message>
<xml_diff>
--- a/data/india/total_bmw_waste.xlsx
+++ b/data/india/total_bmw_waste.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{451844AA-71C2-4CFF-AE47-3B701E0EFD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B42E4B4-9DF8-4F42-8BAE-F183EF509EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4B4E174C-A9DA-4493-A8B8-40B33161D33A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4B4E174C-A9DA-4493-A8B8-40B33161D33A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>3025.41</t>
   </si>
@@ -716,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15A2A4F-ADDD-4801-931F-B7955909B94A}">
   <dimension ref="A1:AJ14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,7 +1771,8 @@
         <v>9.14</v>
       </c>
       <c r="AA14">
-        <v>1.67</v>
+        <f>1.67*30</f>
+        <v>50.099999999999994</v>
       </c>
       <c r="AB14">
         <v>3.87</v>
@@ -1804,4 +1806,3102 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB4B1C6-E8FF-47AD-B663-7CA6948DE709}">
+  <dimension ref="A1:B396"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B2">
+        <f>18.63/30</f>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B31" si="0">18.63/30</f>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>44011</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B32">
+        <f>35.82/31</f>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ref="B33:B62" si="1">35.82/31</f>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>44016</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>44017</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>44020</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>44021</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>44023</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>44024</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>44028</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>44029</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>44030</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>44031</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>44032</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>44033</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>44034</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>44035</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>44036</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>44037</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>44038</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>44039</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>44041</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>44043</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="1"/>
+        <v>1.155483870967742</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B63">
+        <f>41.54/31</f>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>44045</v>
+      </c>
+      <c r="B64">
+        <f t="shared" ref="B64:B93" si="2">41.54/31</f>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B94">
+        <f>63/30</f>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B95">
+        <f t="shared" ref="B95:B123" si="3">63/30</f>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>44079</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B106">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B107">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B108">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B109">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B110">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B111">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B112">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <v>44094</v>
+      </c>
+      <c r="B113">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <v>44095</v>
+      </c>
+      <c r="B114">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <v>44096</v>
+      </c>
+      <c r="B115">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B116">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>44098</v>
+      </c>
+      <c r="B117">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>44099</v>
+      </c>
+      <c r="B118">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>44100</v>
+      </c>
+      <c r="B119">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>44101</v>
+      </c>
+      <c r="B120">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <v>44102</v>
+      </c>
+      <c r="B121">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>44103</v>
+      </c>
+      <c r="B122">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>44104</v>
+      </c>
+      <c r="B123">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>44105</v>
+      </c>
+      <c r="B124">
+        <f>58.652/31</f>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>44106</v>
+      </c>
+      <c r="B125">
+        <f t="shared" ref="B125:B154" si="4">58.652/31</f>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>44107</v>
+      </c>
+      <c r="B126">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
+        <v>44108</v>
+      </c>
+      <c r="B127">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
+        <v>44109</v>
+      </c>
+      <c r="B128">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
+        <v>44110</v>
+      </c>
+      <c r="B129">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
+        <v>44111</v>
+      </c>
+      <c r="B130">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
+        <v>44112</v>
+      </c>
+      <c r="B131">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
+        <v>44113</v>
+      </c>
+      <c r="B132">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
+        <v>44114</v>
+      </c>
+      <c r="B133">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <v>44115</v>
+      </c>
+      <c r="B134">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
+        <v>44116</v>
+      </c>
+      <c r="B135">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
+        <v>44117</v>
+      </c>
+      <c r="B136">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
+        <v>44118</v>
+      </c>
+      <c r="B137">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
+        <v>44119</v>
+      </c>
+      <c r="B138">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
+        <v>44120</v>
+      </c>
+      <c r="B139">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
+        <v>44121</v>
+      </c>
+      <c r="B140">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
+        <v>44122</v>
+      </c>
+      <c r="B141">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
+        <v>44123</v>
+      </c>
+      <c r="B142">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
+        <v>44124</v>
+      </c>
+      <c r="B143">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B144">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="2">
+        <v>44126</v>
+      </c>
+      <c r="B145">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
+        <v>44127</v>
+      </c>
+      <c r="B146">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
+        <v>44128</v>
+      </c>
+      <c r="B147">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
+        <v>44129</v>
+      </c>
+      <c r="B148">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
+        <v>44130</v>
+      </c>
+      <c r="B149">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
+        <v>44131</v>
+      </c>
+      <c r="B150">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <v>44132</v>
+      </c>
+      <c r="B151">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <v>44133</v>
+      </c>
+      <c r="B152">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
+        <v>44134</v>
+      </c>
+      <c r="B153">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <v>44135</v>
+      </c>
+      <c r="B154">
+        <f t="shared" si="4"/>
+        <v>1.8920000000000001</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
+        <v>44136</v>
+      </c>
+      <c r="B155">
+        <f>28.74/30</f>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
+        <v>44137</v>
+      </c>
+      <c r="B156">
+        <f t="shared" ref="B156:B184" si="5">28.74/30</f>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B157">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
+        <v>44139</v>
+      </c>
+      <c r="B158">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
+        <v>44140</v>
+      </c>
+      <c r="B159">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
+        <v>44141</v>
+      </c>
+      <c r="B160">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
+        <v>44142</v>
+      </c>
+      <c r="B161">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
+        <v>44143</v>
+      </c>
+      <c r="B162">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
+        <v>44144</v>
+      </c>
+      <c r="B163">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
+        <v>44145</v>
+      </c>
+      <c r="B164">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
+        <v>44146</v>
+      </c>
+      <c r="B165">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
+        <v>44147</v>
+      </c>
+      <c r="B166">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
+        <v>44148</v>
+      </c>
+      <c r="B167">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B168">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="2">
+        <v>44150</v>
+      </c>
+      <c r="B169">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
+        <v>44151</v>
+      </c>
+      <c r="B170">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
+        <v>44152</v>
+      </c>
+      <c r="B171">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
+        <v>44153</v>
+      </c>
+      <c r="B172">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
+        <v>44154</v>
+      </c>
+      <c r="B173">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
+        <v>44155</v>
+      </c>
+      <c r="B174">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B175">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
+        <v>44157</v>
+      </c>
+      <c r="B176">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
+        <v>44158</v>
+      </c>
+      <c r="B177">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="2">
+        <v>44159</v>
+      </c>
+      <c r="B178">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="2">
+        <v>44160</v>
+      </c>
+      <c r="B179">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="2">
+        <v>44161</v>
+      </c>
+      <c r="B180">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="2">
+        <v>44162</v>
+      </c>
+      <c r="B181">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="2">
+        <v>44163</v>
+      </c>
+      <c r="B182">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="2">
+        <v>44164</v>
+      </c>
+      <c r="B183">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B184">
+        <f t="shared" si="5"/>
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="2">
+        <v>44166</v>
+      </c>
+      <c r="B185">
+        <f>17.11/31</f>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="2">
+        <v>44167</v>
+      </c>
+      <c r="B186">
+        <f t="shared" ref="B186:B215" si="6">17.11/31</f>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="2">
+        <v>44168</v>
+      </c>
+      <c r="B187">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="2">
+        <v>44169</v>
+      </c>
+      <c r="B188">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="2">
+        <v>44170</v>
+      </c>
+      <c r="B189">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
+        <v>44171</v>
+      </c>
+      <c r="B190">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="2">
+        <v>44172</v>
+      </c>
+      <c r="B191">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="2">
+        <v>44173</v>
+      </c>
+      <c r="B192">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B193">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
+        <v>44175</v>
+      </c>
+      <c r="B194">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B195">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="2">
+        <v>44177</v>
+      </c>
+      <c r="B196">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
+        <v>44178</v>
+      </c>
+      <c r="B197">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
+        <v>44179</v>
+      </c>
+      <c r="B198">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B199">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="2">
+        <v>44181</v>
+      </c>
+      <c r="B200">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="2">
+        <v>44182</v>
+      </c>
+      <c r="B201">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B202">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="2">
+        <v>44184</v>
+      </c>
+      <c r="B203">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="2">
+        <v>44185</v>
+      </c>
+      <c r="B204">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="2">
+        <v>44186</v>
+      </c>
+      <c r="B205">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="2">
+        <v>44187</v>
+      </c>
+      <c r="B206">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B207">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="2">
+        <v>44189</v>
+      </c>
+      <c r="B208">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B209">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="2">
+        <v>44191</v>
+      </c>
+      <c r="B210">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="2">
+        <v>44192</v>
+      </c>
+      <c r="B211">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="2">
+        <v>44193</v>
+      </c>
+      <c r="B212">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="2">
+        <v>44194</v>
+      </c>
+      <c r="B213">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="2">
+        <v>44195</v>
+      </c>
+      <c r="B214">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" s="2">
+        <v>44196</v>
+      </c>
+      <c r="B215">
+        <f t="shared" si="6"/>
+        <v>0.55193548387096769</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" s="2">
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" s="2">
+        <v>44198</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" s="2">
+        <v>44199</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" s="2">
+        <v>44200</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" s="2">
+        <v>44201</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" s="2">
+        <v>44202</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" s="2">
+        <v>44203</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" s="2">
+        <v>44204</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" s="2">
+        <v>44205</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="2">
+        <v>44206</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="2">
+        <v>44207</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="2">
+        <v>44208</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="2">
+        <v>44209</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="2">
+        <v>44210</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="2">
+        <v>44211</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="2">
+        <v>44212</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="2">
+        <v>44213</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="2">
+        <v>44214</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="2">
+        <v>44215</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="2">
+        <v>44216</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="2">
+        <v>44217</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="2">
+        <v>44218</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="2">
+        <v>44219</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="2">
+        <v>44220</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="2">
+        <v>44221</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="2">
+        <v>44222</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="2">
+        <v>44223</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="2">
+        <v>44224</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="2">
+        <v>44225</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="2">
+        <v>44226</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="2">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="2">
+        <v>44228</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="2">
+        <v>44229</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="2">
+        <v>44230</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="2">
+        <v>44231</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="2">
+        <v>44232</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="2">
+        <v>44233</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="2">
+        <v>44234</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="2">
+        <v>44235</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="2">
+        <v>44236</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="2">
+        <v>44237</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="2">
+        <v>44238</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="2">
+        <v>44239</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="2">
+        <v>44240</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="2">
+        <v>44241</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="2">
+        <v>44242</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="2">
+        <v>44243</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="2">
+        <v>44244</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="2">
+        <v>44245</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="2">
+        <v>44246</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="2">
+        <v>44247</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="2">
+        <v>44248</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="2">
+        <v>44249</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="2">
+        <v>44250</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="2">
+        <v>44251</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="2">
+        <v>44252</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="2">
+        <v>44253</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="2">
+        <v>44254</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="2">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="2">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="2">
+        <v>44257</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="2">
+        <v>44258</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="2">
+        <v>44259</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="2">
+        <v>44260</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="2">
+        <v>44261</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="2">
+        <v>44262</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" s="2">
+        <v>44263</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="2">
+        <v>44264</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="2">
+        <v>44265</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="2">
+        <v>44266</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="2">
+        <v>44267</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="2">
+        <v>44268</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="2">
+        <v>44269</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="2">
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" s="2">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="2">
+        <v>44272</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="2">
+        <v>44273</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="2">
+        <v>44274</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="2">
+        <v>44275</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="2">
+        <v>44276</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="2">
+        <v>44277</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="2">
+        <v>44278</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" s="2">
+        <v>44279</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" s="2">
+        <v>44280</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="2">
+        <v>44281</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" s="2">
+        <v>44282</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" s="2">
+        <v>44283</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" s="2">
+        <v>44284</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" s="2">
+        <v>44285</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" s="2">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" s="2">
+        <v>44287</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" s="2">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" s="2">
+        <v>44289</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" s="2">
+        <v>44290</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" s="2">
+        <v>44291</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" s="2">
+        <v>44292</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="2">
+        <v>44293</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" s="2">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" s="2">
+        <v>44295</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" s="2">
+        <v>44296</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" s="2">
+        <v>44297</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" s="2">
+        <v>44298</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" s="2">
+        <v>44299</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" s="2">
+        <v>44300</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" s="2">
+        <v>44301</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" s="2">
+        <v>44302</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322" s="2">
+        <v>44303</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323" s="2">
+        <v>44304</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324" s="2">
+        <v>44305</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" s="2">
+        <v>44306</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" s="2">
+        <v>44307</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" s="2">
+        <v>44308</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" s="2">
+        <v>44309</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" s="2">
+        <v>44310</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330" s="2">
+        <v>44311</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331" s="2">
+        <v>44312</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332" s="2">
+        <v>44313</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333" s="2">
+        <v>44314</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334" s="2">
+        <v>44315</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335" s="2">
+        <v>44316</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336" s="2">
+        <v>44317</v>
+      </c>
+      <c r="B336">
+        <f>56.11/31</f>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A337" s="2">
+        <v>44318</v>
+      </c>
+      <c r="B337">
+        <f t="shared" ref="B337:B366" si="7">56.11/31</f>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A338" s="2">
+        <v>44319</v>
+      </c>
+      <c r="B338">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339" s="2">
+        <v>44320</v>
+      </c>
+      <c r="B339">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A340" s="2">
+        <v>44321</v>
+      </c>
+      <c r="B340">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A341" s="2">
+        <v>44322</v>
+      </c>
+      <c r="B341">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342" s="2">
+        <v>44323</v>
+      </c>
+      <c r="B342">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343" s="2">
+        <v>44324</v>
+      </c>
+      <c r="B343">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344" s="2">
+        <v>44325</v>
+      </c>
+      <c r="B344">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345" s="2">
+        <v>44326</v>
+      </c>
+      <c r="B345">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" s="2">
+        <v>44327</v>
+      </c>
+      <c r="B346">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" s="2">
+        <v>44328</v>
+      </c>
+      <c r="B347">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" s="2">
+        <v>44329</v>
+      </c>
+      <c r="B348">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349" s="2">
+        <v>44330</v>
+      </c>
+      <c r="B349">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" s="2">
+        <v>44331</v>
+      </c>
+      <c r="B350">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" s="2">
+        <v>44332</v>
+      </c>
+      <c r="B351">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" s="2">
+        <v>44333</v>
+      </c>
+      <c r="B352">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353" s="2">
+        <v>44334</v>
+      </c>
+      <c r="B353">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354" s="2">
+        <v>44335</v>
+      </c>
+      <c r="B354">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355" s="2">
+        <v>44336</v>
+      </c>
+      <c r="B355">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356" s="2">
+        <v>44337</v>
+      </c>
+      <c r="B356">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" s="2">
+        <v>44338</v>
+      </c>
+      <c r="B357">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" s="2">
+        <v>44339</v>
+      </c>
+      <c r="B358">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359" s="2">
+        <v>44340</v>
+      </c>
+      <c r="B359">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360" s="2">
+        <v>44341</v>
+      </c>
+      <c r="B360">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A361" s="2">
+        <v>44342</v>
+      </c>
+      <c r="B361">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A362" s="2">
+        <v>44343</v>
+      </c>
+      <c r="B362">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363" s="2">
+        <v>44344</v>
+      </c>
+      <c r="B363">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A364" s="2">
+        <v>44345</v>
+      </c>
+      <c r="B364">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365" s="2">
+        <v>44346</v>
+      </c>
+      <c r="B365">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366" s="2">
+        <v>44347</v>
+      </c>
+      <c r="B366">
+        <f t="shared" si="7"/>
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A367" s="2">
+        <v>44348</v>
+      </c>
+      <c r="B367">
+        <f>50.1/30</f>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A368" s="2">
+        <v>44349</v>
+      </c>
+      <c r="B368">
+        <f t="shared" ref="B368:B396" si="8">50.1/30</f>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A369" s="2">
+        <v>44350</v>
+      </c>
+      <c r="B369">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A370" s="2">
+        <v>44351</v>
+      </c>
+      <c r="B370">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371" s="2">
+        <v>44352</v>
+      </c>
+      <c r="B371">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A372" s="2">
+        <v>44353</v>
+      </c>
+      <c r="B372">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A373" s="2">
+        <v>44354</v>
+      </c>
+      <c r="B373">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A374" s="2">
+        <v>44355</v>
+      </c>
+      <c r="B374">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A375" s="2">
+        <v>44356</v>
+      </c>
+      <c r="B375">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A376" s="2">
+        <v>44357</v>
+      </c>
+      <c r="B376">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A377" s="2">
+        <v>44358</v>
+      </c>
+      <c r="B377">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A378" s="2">
+        <v>44359</v>
+      </c>
+      <c r="B378">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A379" s="2">
+        <v>44360</v>
+      </c>
+      <c r="B379">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A380" s="2">
+        <v>44361</v>
+      </c>
+      <c r="B380">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A381" s="2">
+        <v>44362</v>
+      </c>
+      <c r="B381">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A382" s="2">
+        <v>44363</v>
+      </c>
+      <c r="B382">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A383" s="2">
+        <v>44364</v>
+      </c>
+      <c r="B383">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" s="2">
+        <v>44365</v>
+      </c>
+      <c r="B384">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A385" s="2">
+        <v>44366</v>
+      </c>
+      <c r="B385">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A386" s="2">
+        <v>44367</v>
+      </c>
+      <c r="B386">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A387" s="2">
+        <v>44368</v>
+      </c>
+      <c r="B387">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A388" s="2">
+        <v>44369</v>
+      </c>
+      <c r="B388">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A389" s="2">
+        <v>44370</v>
+      </c>
+      <c r="B389">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A390" s="2">
+        <v>44371</v>
+      </c>
+      <c r="B390">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A391" s="2">
+        <v>44372</v>
+      </c>
+      <c r="B391">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A392" s="2">
+        <v>44373</v>
+      </c>
+      <c r="B392">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A393" s="2">
+        <v>44374</v>
+      </c>
+      <c r="B393">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A394" s="2">
+        <v>44375</v>
+      </c>
+      <c r="B394">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A395" s="2">
+        <v>44376</v>
+      </c>
+      <c r="B395">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A396" s="2">
+        <v>44377</v>
+      </c>
+      <c r="B396">
+        <f t="shared" si="8"/>
+        <v>1.6700000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>